<commit_message>
renamed column as label_RQ1
</commit_message>
<xml_diff>
--- a/results_analysis/RQ1/label_undetermined_responses/crows_gpt3_completions_RQ1_label_undeter.xlsx
+++ b/results_analysis/RQ1/label_undetermined_responses/crows_gpt3_completions_RQ1_label_undeter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/461cf661edc880ea/Documentos/GitHub/Thesis/results_analysis/RQ1/label_undetermined_responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="387" documentId="11_0D9540EE266B093C412D4C08052D3833786CCDC9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F3352E3-6092-45D8-AF68-540C123123BF}"/>
+  <xr:revisionPtr revIDLastSave="389" documentId="11_0D9540EE266B093C412D4C08052D3833786CCDC9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EFA38CD-0A66-405E-9E26-0E5A04B70901}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17887,10 +17887,10 @@
     <t>Bad intentions detection</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
     <t>Avoid (un)targeted term</t>
+  </si>
+  <si>
+    <t>label_RQ1</t>
   </si>
 </sst>
 </file>
@@ -18279,7 +18279,7 @@
   <dimension ref="A1:J1509"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18316,7 +18316,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>4948</v>
+        <v>4949</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -32458,7 +32458,7 @@
         <v>4942</v>
       </c>
       <c r="J478" t="s">
-        <v>4949</v>
+        <v>4948</v>
       </c>
     </row>
     <row r="479" spans="1:10" x14ac:dyDescent="0.45">
@@ -48742,7 +48742,7 @@
         <v>4942</v>
       </c>
       <c r="J1027" t="s">
-        <v>4949</v>
+        <v>4948</v>
       </c>
     </row>
     <row r="1028" spans="1:10" x14ac:dyDescent="0.45">
@@ -54666,7 +54666,7 @@
         <v>4942</v>
       </c>
       <c r="J1226" t="s">
-        <v>4949</v>
+        <v>4948</v>
       </c>
     </row>
     <row r="1227" spans="1:10" x14ac:dyDescent="0.45">
@@ -63078,11 +63078,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1509" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J1509">
-      <sortCondition ref="A1:A1509"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:J1509" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1437 J1505:J1509" xr:uid="{8A233681-FB80-46D8-87F8-CFCBCAAF0523}">
       <formula1>$M$2:$M$10</formula1>

</xml_diff>